<commit_message>
added twitter sentiment analysis
</commit_message>
<xml_diff>
--- a/Excel reports/adjusted_df_news.xlsx
+++ b/Excel reports/adjusted_df_news.xlsx
@@ -447,7 +447,7 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>APISentiment</t>
+          <t>CombinedVaderSentiment</t>
         </is>
       </c>
     </row>
@@ -456,7 +456,7 @@
         <v>44543</v>
       </c>
       <c r="B2" t="n">
-        <v>0.963</v>
+        <v>0.959</v>
       </c>
     </row>
     <row r="3">
@@ -464,7 +464,7 @@
         <v>44550</v>
       </c>
       <c r="B3" t="n">
-        <v>0.548</v>
+        <v>0.56335</v>
       </c>
     </row>
     <row r="4">
@@ -472,7 +472,7 @@
         <v>44557</v>
       </c>
       <c r="B4" t="n">
-        <v>0.891</v>
+        <v>0.5781000000000001</v>
       </c>
     </row>
     <row r="5">
@@ -480,7 +480,7 @@
         <v>44564</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9350000000000001</v>
+        <v>0.852</v>
       </c>
     </row>
     <row r="6">
@@ -488,7 +488,7 @@
         <v>44571</v>
       </c>
       <c r="B6" t="n">
-        <v>0.9944999999999999</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="7">
@@ -496,7 +496,7 @@
         <v>44578</v>
       </c>
       <c r="B7" t="n">
-        <v>0.993</v>
+        <v>0.9924999999999999</v>
       </c>
     </row>
     <row r="8">
@@ -504,7 +504,7 @@
         <v>44585</v>
       </c>
       <c r="B8" t="n">
-        <v>0.994</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="9">
@@ -512,7 +512,7 @@
         <v>44592</v>
       </c>
       <c r="B9" t="n">
-        <v>0.994</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="10">
@@ -520,7 +520,7 @@
         <v>44599</v>
       </c>
       <c r="B10" t="n">
-        <v>0.976</v>
+        <v>0.986</v>
       </c>
     </row>
     <row r="11">
@@ -528,7 +528,7 @@
         <v>44606</v>
       </c>
       <c r="B11" t="n">
-        <v>0.9804999999999999</v>
+        <v>0.8704499999999999</v>
       </c>
     </row>
     <row r="12">
@@ -536,7 +536,7 @@
         <v>44613</v>
       </c>
       <c r="B12" t="n">
-        <v>0.9944999999999999</v>
+        <v>0.9975000000000001</v>
       </c>
     </row>
     <row r="13">
@@ -544,7 +544,7 @@
         <v>44620</v>
       </c>
       <c r="B13" t="n">
-        <v>0.9550000000000001</v>
+        <v>1.1598</v>
       </c>
     </row>
     <row r="14">
@@ -552,7 +552,7 @@
         <v>44627</v>
       </c>
       <c r="B14" t="n">
-        <v>0.996</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="15">
@@ -560,7 +560,7 @@
         <v>44634</v>
       </c>
       <c r="B15" t="n">
-        <v>0.75</v>
+        <v>0.19515</v>
       </c>
     </row>
     <row r="16">
@@ -568,7 +568,7 @@
         <v>44641</v>
       </c>
       <c r="B16" t="n">
-        <v>0.9655</v>
+        <v>0.86225</v>
       </c>
     </row>
     <row r="17">
@@ -576,7 +576,7 @@
         <v>44648</v>
       </c>
       <c r="B17" t="n">
-        <v>0.96</v>
+        <v>0.957</v>
       </c>
     </row>
     <row r="18">
@@ -584,7 +584,7 @@
         <v>44655</v>
       </c>
       <c r="B18" t="n">
-        <v>0.993</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="19">
@@ -600,7 +600,7 @@
         <v>44669</v>
       </c>
       <c r="B20" t="n">
-        <v>0.977</v>
+        <v>0.9804999999999999</v>
       </c>
     </row>
     <row r="21">
@@ -608,7 +608,7 @@
         <v>44676</v>
       </c>
       <c r="B21" t="n">
-        <v>0.9675</v>
+        <v>0.9895</v>
       </c>
     </row>
     <row r="22">
@@ -616,7 +616,7 @@
         <v>44683</v>
       </c>
       <c r="B22" t="n">
-        <v>0.998</v>
+        <v>1.0248</v>
       </c>
     </row>
     <row r="23">
@@ -640,7 +640,7 @@
         <v>44704</v>
       </c>
       <c r="B25" t="n">
-        <v>0.991</v>
+        <v>0.86465</v>
       </c>
     </row>
     <row r="26">
@@ -648,7 +648,7 @@
         <v>44711</v>
       </c>
       <c r="B26" t="n">
-        <v>0.9955000000000001</v>
+        <v>0.996</v>
       </c>
     </row>
     <row r="27">
@@ -664,7 +664,7 @@
         <v>44725</v>
       </c>
       <c r="B28" t="n">
-        <v>0.98</v>
+        <v>0.957</v>
       </c>
     </row>
     <row r="29">
@@ -672,7 +672,7 @@
         <v>44732</v>
       </c>
       <c r="B29" t="n">
-        <v>0.95</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="30">
@@ -680,7 +680,7 @@
         <v>44739</v>
       </c>
       <c r="B30" t="n">
-        <v>0.988</v>
+        <v>0.993</v>
       </c>
     </row>
     <row r="31">
@@ -688,7 +688,7 @@
         <v>44746</v>
       </c>
       <c r="B31" t="n">
-        <v>0.9935</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="32">
@@ -696,7 +696,7 @@
         <v>44753</v>
       </c>
       <c r="B32" t="n">
-        <v>0.996</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="33">
@@ -712,7 +712,7 @@
         <v>44767</v>
       </c>
       <c r="B34" t="n">
-        <v>0.959</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="35">
@@ -720,7 +720,7 @@
         <v>44774</v>
       </c>
       <c r="B35" t="n">
-        <v>0.992</v>
+        <v>0.90655</v>
       </c>
     </row>
     <row r="36">
@@ -728,7 +728,7 @@
         <v>44781</v>
       </c>
       <c r="B36" t="n">
-        <v>0.985</v>
+        <v>0.7800499999999999</v>
       </c>
     </row>
     <row r="37">
@@ -736,7 +736,7 @@
         <v>44788</v>
       </c>
       <c r="B37" t="n">
-        <v>0.985</v>
+        <v>0.9955000000000001</v>
       </c>
     </row>
     <row r="38">
@@ -744,7 +744,7 @@
         <v>44795</v>
       </c>
       <c r="B38" t="n">
-        <v>0.991</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="39">
@@ -752,7 +752,7 @@
         <v>44802</v>
       </c>
       <c r="B39" t="n">
-        <v>0.978</v>
+        <v>0.9924999999999999</v>
       </c>
     </row>
     <row r="40">

</xml_diff>

<commit_message>
added testing pyscript, with enhanced functionality
</commit_message>
<xml_diff>
--- a/Excel reports/adjusted_df_news.xlsx
+++ b/Excel reports/adjusted_df_news.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B64"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,135 +453,135 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>43976</v>
+        <v>44543</v>
       </c>
       <c r="B2" t="n">
-        <v>0.996</v>
+        <v>1.3612</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44060</v>
+        <v>44550</v>
       </c>
       <c r="B3" t="n">
-        <v>1.2013</v>
+        <v>0.56335</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44067</v>
+        <v>44557</v>
       </c>
       <c r="B4" t="n">
-        <v>0.996</v>
+        <v>0.5781000000000001</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44158</v>
+        <v>44564</v>
       </c>
       <c r="B5" t="n">
-        <v>1.1995</v>
+        <v>0.852</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44165</v>
+        <v>44571</v>
       </c>
       <c r="B6" t="n">
-        <v>0.6774</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44172</v>
+        <v>44578</v>
       </c>
       <c r="B7" t="n">
-        <v>0.997</v>
+        <v>0.9924999999999999</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44179</v>
+        <v>44585</v>
       </c>
       <c r="B8" t="n">
-        <v>1.4364</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44186</v>
+        <v>44592</v>
       </c>
       <c r="B9" t="n">
-        <v>1.4394</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44193</v>
+        <v>44599</v>
       </c>
       <c r="B10" t="n">
-        <v>0.796</v>
+        <v>0.986</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44207</v>
+        <v>44606</v>
       </c>
       <c r="B11" t="n">
-        <v>0.982</v>
+        <v>0.8704499999999999</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44214</v>
+        <v>44613</v>
       </c>
       <c r="B12" t="n">
-        <v>0.994</v>
+        <v>0.9975000000000001</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44221</v>
+        <v>44620</v>
       </c>
       <c r="B13" t="n">
-        <v>0.988</v>
+        <v>1.1598</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44249</v>
+        <v>44627</v>
       </c>
       <c r="B14" t="n">
-        <v>0.168</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44263</v>
+        <v>44634</v>
       </c>
       <c r="B15" t="n">
-        <v>1.6219</v>
+        <v>0.19515</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44277</v>
+        <v>44641</v>
       </c>
       <c r="B16" t="n">
-        <v>0.645</v>
+        <v>0.86225</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>44298</v>
+        <v>44648</v>
       </c>
       <c r="B17" t="n">
-        <v>1.1303</v>
+        <v>0.957</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>44305</v>
+        <v>44655</v>
       </c>
       <c r="B18" t="n">
         <v>0.998</v>
@@ -589,370 +589,194 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>44319</v>
+        <v>44662</v>
       </c>
       <c r="B19" t="n">
-        <v>0.996</v>
+        <v>0.967</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>44333</v>
+        <v>44669</v>
       </c>
       <c r="B20" t="n">
-        <v>0.8464499999999999</v>
+        <v>0.9804999999999999</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>44347</v>
+        <v>44676</v>
       </c>
       <c r="B21" t="n">
-        <v>1.0171</v>
+        <v>0.9895</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>44361</v>
+        <v>44683</v>
       </c>
       <c r="B22" t="n">
-        <v>0.987</v>
+        <v>1.0248</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>44375</v>
+        <v>44690</v>
       </c>
       <c r="B23" t="n">
-        <v>0.546</v>
+        <v>0.679</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>44382</v>
+        <v>44697</v>
       </c>
       <c r="B24" t="n">
-        <v>0.976</v>
+        <v>0.999</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>44389</v>
+        <v>44704</v>
       </c>
       <c r="B25" t="n">
-        <v>1.4929</v>
+        <v>0.86465</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>44396</v>
+        <v>44711</v>
       </c>
       <c r="B26" t="n">
-        <v>0.5096000000000001</v>
+        <v>0.996</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>44403</v>
+        <v>44718</v>
       </c>
       <c r="B27" t="n">
-        <v>0.8149</v>
+        <v>0.956</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>44410</v>
+        <v>44725</v>
       </c>
       <c r="B28" t="n">
-        <v>0.79545</v>
+        <v>0.957</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>44417</v>
+        <v>44732</v>
       </c>
       <c r="B29" t="n">
-        <v>0.997</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>44424</v>
+        <v>44739</v>
       </c>
       <c r="B30" t="n">
-        <v>1.0642</v>
+        <v>0.993</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>44431</v>
+        <v>44746</v>
       </c>
       <c r="B31" t="n">
-        <v>1.08715</v>
+        <v>0.98</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>44452</v>
+        <v>44753</v>
       </c>
       <c r="B32" t="n">
-        <v>1.4314</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>44466</v>
+        <v>44760</v>
       </c>
       <c r="B33" t="n">
-        <v>0.796</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>44473</v>
+        <v>44767</v>
       </c>
       <c r="B34" t="n">
-        <v>1.6249</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>44487</v>
+        <v>44774</v>
       </c>
       <c r="B35" t="n">
-        <v>0.8379</v>
+        <v>0.90655</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>44494</v>
+        <v>44781</v>
       </c>
       <c r="B36" t="n">
-        <v>0.997</v>
+        <v>0.7800499999999999</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>44501</v>
+        <v>44788</v>
       </c>
       <c r="B37" t="n">
-        <v>0.999</v>
+        <v>0.9955000000000001</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>44508</v>
+        <v>44795</v>
       </c>
       <c r="B38" t="n">
-        <v>1.24485</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>44543</v>
+        <v>44802</v>
       </c>
       <c r="B39" t="n">
-        <v>0.998</v>
+        <v>0.9924999999999999</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>44564</v>
+        <v>44809</v>
       </c>
       <c r="B40" t="n">
-        <v>0.872</v>
+        <v>0.986</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>44571</v>
+        <v>44816</v>
       </c>
       <c r="B41" t="n">
-        <v>1.291</v>
+        <v>0.993</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>44585</v>
+        <v>44823</v>
       </c>
       <c r="B42" t="n">
-        <v>1.4452</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="2" t="n">
-        <v>44592</v>
-      </c>
-      <c r="B43" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="2" t="n">
-        <v>44599</v>
-      </c>
-      <c r="B44" t="n">
-        <v>0.992</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="2" t="n">
-        <v>44620</v>
-      </c>
-      <c r="B45" t="n">
-        <v>0.992</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="2" t="n">
-        <v>44627</v>
-      </c>
-      <c r="B46" t="n">
-        <v>1.4859</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="2" t="n">
-        <v>44634</v>
-      </c>
-      <c r="B47" t="n">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="2" t="n">
-        <v>44641</v>
-      </c>
-      <c r="B48" t="n">
-        <v>0.996</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="2" t="n">
-        <v>44648</v>
-      </c>
-      <c r="B49" t="n">
-        <v>1.115</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="2" t="n">
-        <v>44669</v>
-      </c>
-      <c r="B50" t="n">
         <v>0.998</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="2" t="n">
-        <v>44676</v>
-      </c>
-      <c r="B51" t="n">
-        <v>0.995</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="2" t="n">
-        <v>44683</v>
-      </c>
-      <c r="B52" t="n">
-        <v>1.28395</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="2" t="n">
-        <v>44704</v>
-      </c>
-      <c r="B53" t="n">
-        <v>0.8369</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="2" t="n">
-        <v>44711</v>
-      </c>
-      <c r="B54" t="n">
-        <v>1.461</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="2" t="n">
-        <v>44718</v>
-      </c>
-      <c r="B55" t="n">
-        <v>0.375</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="2" t="n">
-        <v>44732</v>
-      </c>
-      <c r="B56" t="n">
-        <v>1.013</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="2" t="n">
-        <v>44739</v>
-      </c>
-      <c r="B57" t="n">
-        <v>0.796</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="2" t="n">
-        <v>44746</v>
-      </c>
-      <c r="B58" t="n">
-        <v>0.9865999999999999</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="2" t="n">
-        <v>44760</v>
-      </c>
-      <c r="B59" t="n">
-        <v>0.986</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="2" t="n">
-        <v>44767</v>
-      </c>
-      <c r="B60" t="n">
-        <v>-0.081</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="2" t="n">
-        <v>44774</v>
-      </c>
-      <c r="B61" t="n">
-        <v>0.995</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="2" t="n">
-        <v>44781</v>
-      </c>
-      <c r="B62" t="n">
-        <v>1.2152</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="2" t="n">
-        <v>44795</v>
-      </c>
-      <c r="B63" t="n">
-        <v>1.162</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="2" t="n">
-        <v>44809</v>
-      </c>
-      <c r="B64" t="n">
-        <v>1.6466</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added additional API call to get data
</commit_message>
<xml_diff>
--- a/Excel reports/adjusted_df_news.xlsx
+++ b/Excel reports/adjusted_df_news.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B229"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,263 +453,263 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44543</v>
+        <v>44547</v>
       </c>
       <c r="B2" t="n">
-        <v>1.3612</v>
+        <v>0.4602</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44550</v>
+        <v>44549</v>
       </c>
       <c r="B3" t="n">
-        <v>0.56335</v>
+        <v>1.3612</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44557</v>
+        <v>44550</v>
       </c>
       <c r="B4" t="n">
-        <v>0.5781000000000001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44564</v>
+        <v>44551</v>
       </c>
       <c r="B5" t="n">
-        <v>0.852</v>
+        <v>-0.0516</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44571</v>
+        <v>44552</v>
       </c>
       <c r="B6" t="n">
-        <v>0.995</v>
+        <v>0.103</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44578</v>
+        <v>44553</v>
       </c>
       <c r="B7" t="n">
-        <v>0.9924999999999999</v>
+        <v>0.6021000000000001</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44585</v>
+        <v>44554</v>
       </c>
       <c r="B8" t="n">
-        <v>0.995</v>
+        <v>1.3604</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>44592</v>
+        <v>44555</v>
       </c>
       <c r="B9" t="n">
-        <v>0.995</v>
+        <v>1.4185</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
-        <v>44599</v>
+        <v>44557</v>
       </c>
       <c r="B10" t="n">
-        <v>0.986</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
-        <v>44606</v>
+        <v>44558</v>
       </c>
       <c r="B11" t="n">
-        <v>0.8704499999999999</v>
+        <v>0.8051</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
-        <v>44613</v>
+        <v>44559</v>
       </c>
       <c r="B12" t="n">
-        <v>0.9975000000000001</v>
+        <v>0.2371</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
-        <v>44620</v>
+        <v>44560</v>
       </c>
       <c r="B13" t="n">
-        <v>1.1598</v>
+        <v>0.995</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44627</v>
+        <v>44561</v>
       </c>
       <c r="B14" t="n">
-        <v>0.998</v>
+        <v>0.32955</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
-        <v>44634</v>
+        <v>44562</v>
       </c>
       <c r="B15" t="n">
-        <v>0.19515</v>
+        <v>-0.02459999999999996</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
-        <v>44641</v>
+        <v>44563</v>
       </c>
       <c r="B16" t="n">
-        <v>0.86225</v>
+        <v>0.798</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
-        <v>44648</v>
+        <v>44564</v>
       </c>
       <c r="B17" t="n">
-        <v>0.957</v>
+        <v>-0.01764999999999994</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
-        <v>44655</v>
+        <v>44565</v>
       </c>
       <c r="B18" t="n">
-        <v>0.998</v>
+        <v>0.63315</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
-        <v>44662</v>
+        <v>44566</v>
       </c>
       <c r="B19" t="n">
-        <v>0.967</v>
+        <v>1.4996</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
-        <v>44669</v>
+        <v>44567</v>
       </c>
       <c r="B20" t="n">
-        <v>0.9804999999999999</v>
+        <v>-0.12175</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
-        <v>44676</v>
+        <v>44568</v>
       </c>
       <c r="B21" t="n">
-        <v>0.9895</v>
+        <v>0.92</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
-        <v>44683</v>
+        <v>44571</v>
       </c>
       <c r="B22" t="n">
-        <v>1.0248</v>
+        <v>0.988</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
-        <v>44690</v>
+        <v>44572</v>
       </c>
       <c r="B23" t="n">
-        <v>0.679</v>
+        <v>0.66415</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
-        <v>44697</v>
+        <v>44573</v>
       </c>
       <c r="B24" t="n">
-        <v>0.999</v>
+        <v>0.997</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
-        <v>44704</v>
+        <v>44574</v>
       </c>
       <c r="B25" t="n">
-        <v>0.86465</v>
+        <v>0.992</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
-        <v>44711</v>
+        <v>44575</v>
       </c>
       <c r="B26" t="n">
-        <v>0.996</v>
+        <v>1.5056</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
-        <v>44718</v>
+        <v>44577</v>
       </c>
       <c r="B27" t="n">
-        <v>0.956</v>
+        <v>0.5570000000000001</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
-        <v>44725</v>
+        <v>44578</v>
       </c>
       <c r="B28" t="n">
-        <v>0.957</v>
+        <v>1.3412</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
-        <v>44732</v>
+        <v>44579</v>
       </c>
       <c r="B29" t="n">
-        <v>0.988</v>
+        <v>0.994</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
-        <v>44739</v>
+        <v>44580</v>
       </c>
       <c r="B30" t="n">
-        <v>0.993</v>
+        <v>1.4899</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
-        <v>44746</v>
+        <v>44581</v>
       </c>
       <c r="B31" t="n">
-        <v>0.98</v>
+        <v>0.9384</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
-        <v>44753</v>
+        <v>44582</v>
       </c>
       <c r="B32" t="n">
-        <v>0.998</v>
+        <v>0.992</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
-        <v>44760</v>
+        <v>44585</v>
       </c>
       <c r="B33" t="n">
-        <v>0.997</v>
+        <v>0.984</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
-        <v>44767</v>
+        <v>44586</v>
       </c>
       <c r="B34" t="n">
         <v>0.995</v>
@@ -717,66 +717,1562 @@
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
-        <v>44774</v>
+        <v>44587</v>
       </c>
       <c r="B35" t="n">
-        <v>0.90655</v>
+        <v>1.24545</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
-        <v>44781</v>
+        <v>44588</v>
       </c>
       <c r="B36" t="n">
-        <v>0.7800499999999999</v>
+        <v>0.9984999999999999</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="n">
-        <v>44788</v>
+        <v>44589</v>
       </c>
       <c r="B37" t="n">
-        <v>0.9955000000000001</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="n">
-        <v>44795</v>
+        <v>44590</v>
       </c>
       <c r="B38" t="n">
-        <v>0.99</v>
+        <v>0.3397</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2" t="n">
-        <v>44802</v>
+        <v>44591</v>
       </c>
       <c r="B39" t="n">
-        <v>0.9924999999999999</v>
+        <v>1.1713</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
-        <v>44809</v>
+        <v>44592</v>
       </c>
       <c r="B40" t="n">
-        <v>0.986</v>
+        <v>0.766</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="n">
-        <v>44816</v>
+        <v>44593</v>
       </c>
       <c r="B41" t="n">
-        <v>0.993</v>
+        <v>0.992</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
-        <v>44823</v>
+        <v>44594</v>
       </c>
       <c r="B42" t="n">
         <v>0.998</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="n">
+        <v>44595</v>
+      </c>
+      <c r="B43" t="n">
+        <v>0.983</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="n">
+        <v>44596</v>
+      </c>
+      <c r="B44" t="n">
+        <v>0.989</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="n">
+        <v>44598</v>
+      </c>
+      <c r="B45" t="n">
+        <v>1.1889</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="n">
+        <v>44599</v>
+      </c>
+      <c r="B46" t="n">
+        <v>-0.1365</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="n">
+        <v>44600</v>
+      </c>
+      <c r="B47" t="n">
+        <v>0.9895</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="n">
+        <v>44601</v>
+      </c>
+      <c r="B48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="n">
+        <v>44602</v>
+      </c>
+      <c r="B49" t="n">
+        <v>0.82285</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="n">
+        <v>44603</v>
+      </c>
+      <c r="B50" t="n">
+        <v>1.12975</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="n">
+        <v>44606</v>
+      </c>
+      <c r="B51" t="n">
+        <v>0.5952</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="n">
+        <v>44607</v>
+      </c>
+      <c r="B52" t="n">
+        <v>-0.875</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="n">
+        <v>44608</v>
+      </c>
+      <c r="B53" t="n">
+        <v>0.992</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="n">
+        <v>44609</v>
+      </c>
+      <c r="B54" t="n">
+        <v>0.908</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="2" t="n">
+        <v>44610</v>
+      </c>
+      <c r="B55" t="n">
+        <v>0.96765</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="2" t="n">
+        <v>44611</v>
+      </c>
+      <c r="B56" t="n">
+        <v>1.3376</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="2" t="n">
+        <v>44612</v>
+      </c>
+      <c r="B57" t="n">
+        <v>1.2013</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="2" t="n">
+        <v>44613</v>
+      </c>
+      <c r="B58" t="n">
+        <v>0.992</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="2" t="n">
+        <v>44614</v>
+      </c>
+      <c r="B59" t="n">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="2" t="n">
+        <v>44615</v>
+      </c>
+      <c r="B60" t="n">
+        <v>0.9984999999999999</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="2" t="n">
+        <v>44616</v>
+      </c>
+      <c r="B61" t="n">
+        <v>1.4181</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="2" t="n">
+        <v>44617</v>
+      </c>
+      <c r="B62" t="n">
+        <v>0.8269</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="2" t="n">
+        <v>44618</v>
+      </c>
+      <c r="B63" t="n">
+        <v>0.8179999999999999</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="2" t="n">
+        <v>44620</v>
+      </c>
+      <c r="B64" t="n">
+        <v>0.3519</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="2" t="n">
+        <v>44621</v>
+      </c>
+      <c r="B65" t="n">
+        <v>1.1293</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="2" t="n">
+        <v>44622</v>
+      </c>
+      <c r="B66" t="n">
+        <v>0.6143000000000001</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="2" t="n">
+        <v>44623</v>
+      </c>
+      <c r="B67" t="n">
+        <v>0.167</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="2" t="n">
+        <v>44624</v>
+      </c>
+      <c r="B68" t="n">
+        <v>1.45285</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="2" t="n">
+        <v>44625</v>
+      </c>
+      <c r="B69" t="n">
+        <v>0.681</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="2" t="n">
+        <v>44627</v>
+      </c>
+      <c r="B70" t="n">
+        <v>1.23185</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="2" t="n">
+        <v>44628</v>
+      </c>
+      <c r="B71" t="n">
+        <v>-0.7606999999999999</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="2" t="n">
+        <v>44629</v>
+      </c>
+      <c r="B72" t="n">
+        <v>1.2253</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="2" t="n">
+        <v>44630</v>
+      </c>
+      <c r="B73" t="n">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="2" t="n">
+        <v>44631</v>
+      </c>
+      <c r="B74" t="n">
+        <v>0.989</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="2" t="n">
+        <v>44632</v>
+      </c>
+      <c r="B75" t="n">
+        <v>-1.4019</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="2" t="n">
+        <v>44634</v>
+      </c>
+      <c r="B76" t="n">
+        <v>0.32155</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="2" t="n">
+        <v>44635</v>
+      </c>
+      <c r="B77" t="n">
+        <v>-0.1628000000000001</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="2" t="n">
+        <v>44636</v>
+      </c>
+      <c r="B78" t="n">
+        <v>0.983</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="2" t="n">
+        <v>44637</v>
+      </c>
+      <c r="B79" t="n">
+        <v>0.16665</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="2" t="n">
+        <v>44638</v>
+      </c>
+      <c r="B80" t="n">
+        <v>1.5789</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="n">
+        <v>44641</v>
+      </c>
+      <c r="B81" t="n">
+        <v>0.18315</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="2" t="n">
+        <v>44642</v>
+      </c>
+      <c r="B82" t="n">
+        <v>0.9361999999999999</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="2" t="n">
+        <v>44643</v>
+      </c>
+      <c r="B83" t="n">
+        <v>0.68145</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="2" t="n">
+        <v>44644</v>
+      </c>
+      <c r="B84" t="n">
+        <v>1.4599</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="2" t="n">
+        <v>44645</v>
+      </c>
+      <c r="B85" t="n">
+        <v>0.616</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="2" t="n">
+        <v>44648</v>
+      </c>
+      <c r="B86" t="n">
+        <v>0.992</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="2" t="n">
+        <v>44649</v>
+      </c>
+      <c r="B87" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="2" t="n">
+        <v>44650</v>
+      </c>
+      <c r="B88" t="n">
+        <v>-1.798</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="2" t="n">
+        <v>44651</v>
+      </c>
+      <c r="B89" t="n">
+        <v>0.33765</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="2" t="n">
+        <v>44652</v>
+      </c>
+      <c r="B90" t="n">
+        <v>0.957</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="2" t="n">
+        <v>44653</v>
+      </c>
+      <c r="B91" t="n">
+        <v>1.7269</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="2" t="n">
+        <v>44655</v>
+      </c>
+      <c r="B92" t="n">
+        <v>0.9715</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="2" t="n">
+        <v>44656</v>
+      </c>
+      <c r="B93" t="n">
+        <v>1.45455</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="2" t="n">
+        <v>44657</v>
+      </c>
+      <c r="B94" t="n">
+        <v>1.09665</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="2" t="n">
+        <v>44658</v>
+      </c>
+      <c r="B95" t="n">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="2" t="n">
+        <v>44659</v>
+      </c>
+      <c r="B96" t="n">
+        <v>0.987</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="2" t="n">
+        <v>44662</v>
+      </c>
+      <c r="B97" t="n">
+        <v>0.007</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="2" t="n">
+        <v>44663</v>
+      </c>
+      <c r="B98" t="n">
+        <v>0.985</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="2" t="n">
+        <v>44664</v>
+      </c>
+      <c r="B99" t="n">
+        <v>0.76305</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="2" t="n">
+        <v>44665</v>
+      </c>
+      <c r="B100" t="n">
+        <v>1.244</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="2" t="n">
+        <v>44666</v>
+      </c>
+      <c r="B101" t="n">
+        <v>0.9964999999999999</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="2" t="n">
+        <v>44669</v>
+      </c>
+      <c r="B102" t="n">
+        <v>-1.3938</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="2" t="n">
+        <v>44670</v>
+      </c>
+      <c r="B103" t="n">
+        <v>0.5765</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="2" t="n">
+        <v>44671</v>
+      </c>
+      <c r="B104" t="n">
+        <v>1.329</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="2" t="n">
+        <v>44672</v>
+      </c>
+      <c r="B105" t="n">
+        <v>0.76835</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="2" t="n">
+        <v>44673</v>
+      </c>
+      <c r="B106" t="n">
+        <v>0.926</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="2" t="n">
+        <v>44676</v>
+      </c>
+      <c r="B107" t="n">
+        <v>1.5257</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="2" t="n">
+        <v>44677</v>
+      </c>
+      <c r="B108" t="n">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="2" t="n">
+        <v>44678</v>
+      </c>
+      <c r="B109" t="n">
+        <v>1.123</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="2" t="n">
+        <v>44679</v>
+      </c>
+      <c r="B110" t="n">
+        <v>0.505</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="2" t="n">
+        <v>44680</v>
+      </c>
+      <c r="B111" t="n">
+        <v>0.026</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="2" t="n">
+        <v>44683</v>
+      </c>
+      <c r="B112" t="n">
+        <v>1.4394</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="2" t="n">
+        <v>44684</v>
+      </c>
+      <c r="B113" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="2" t="n">
+        <v>44685</v>
+      </c>
+      <c r="B114" t="n">
+        <v>1.136</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="2" t="n">
+        <v>44686</v>
+      </c>
+      <c r="B115" t="n">
+        <v>-0.0518</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="2" t="n">
+        <v>44687</v>
+      </c>
+      <c r="B116" t="n">
+        <v>1.25835</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="2" t="n">
+        <v>44690</v>
+      </c>
+      <c r="B117" t="n">
+        <v>1.4384</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="2" t="n">
+        <v>44691</v>
+      </c>
+      <c r="B118" t="n">
+        <v>-0.1874</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="2" t="n">
+        <v>44692</v>
+      </c>
+      <c r="B119" t="n">
+        <v>-0.3163499999999999</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="2" t="n">
+        <v>44693</v>
+      </c>
+      <c r="B120" t="n">
+        <v>-0.47385</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="2" t="n">
+        <v>44694</v>
+      </c>
+      <c r="B121" t="n">
+        <v>1.296</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="2" t="n">
+        <v>44697</v>
+      </c>
+      <c r="B122" t="n">
+        <v>1.3808</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="2" t="n">
+        <v>44698</v>
+      </c>
+      <c r="B123" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="2" t="n">
+        <v>44699</v>
+      </c>
+      <c r="B124" t="n">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="2" t="n">
+        <v>44700</v>
+      </c>
+      <c r="B125" t="n">
+        <v>1.1581</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="2" t="n">
+        <v>44701</v>
+      </c>
+      <c r="B126" t="n">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="2" t="n">
+        <v>44702</v>
+      </c>
+      <c r="B127" t="n">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="2" t="n">
+        <v>44704</v>
+      </c>
+      <c r="B128" t="n">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="2" t="n">
+        <v>44705</v>
+      </c>
+      <c r="B129" t="n">
+        <v>0.985</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="2" t="n">
+        <v>44706</v>
+      </c>
+      <c r="B130" t="n">
+        <v>0.5393000000000001</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="2" t="n">
+        <v>44707</v>
+      </c>
+      <c r="B131" t="n">
+        <v>-0.1733</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="2" t="n">
+        <v>44708</v>
+      </c>
+      <c r="B132" t="n">
+        <v>0.9924999999999999</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="2" t="n">
+        <v>44711</v>
+      </c>
+      <c r="B133" t="n">
+        <v>1.6369</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="2" t="n">
+        <v>44712</v>
+      </c>
+      <c r="B134" t="n">
+        <v>0.527</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="2" t="n">
+        <v>44713</v>
+      </c>
+      <c r="B135" t="n">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="2" t="n">
+        <v>44714</v>
+      </c>
+      <c r="B136" t="n">
+        <v>0.599</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="2" t="n">
+        <v>44715</v>
+      </c>
+      <c r="B137" t="n">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="2" t="n">
+        <v>44717</v>
+      </c>
+      <c r="B138" t="n">
+        <v>0.2732</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="2" t="n">
+        <v>44718</v>
+      </c>
+      <c r="B139" t="n">
+        <v>0.2838</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="2" t="n">
+        <v>44719</v>
+      </c>
+      <c r="B140" t="n">
+        <v>0.9715</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="2" t="n">
+        <v>44720</v>
+      </c>
+      <c r="B141" t="n">
+        <v>0.8324</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="2" t="n">
+        <v>44721</v>
+      </c>
+      <c r="B142" t="n">
+        <v>0.989</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="2" t="n">
+        <v>44722</v>
+      </c>
+      <c r="B143" t="n">
+        <v>-0.3815</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="2" t="n">
+        <v>44723</v>
+      </c>
+      <c r="B144" t="n">
+        <v>0.6369</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="2" t="n">
+        <v>44725</v>
+      </c>
+      <c r="B145" t="n">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="2" t="n">
+        <v>44726</v>
+      </c>
+      <c r="B146" t="n">
+        <v>0.4713999999999999</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="2" t="n">
+        <v>44727</v>
+      </c>
+      <c r="B147" t="n">
+        <v>0.957</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="2" t="n">
+        <v>44728</v>
+      </c>
+      <c r="B148" t="n">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="2" t="n">
+        <v>44729</v>
+      </c>
+      <c r="B149" t="n">
+        <v>0.8734500000000001</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="2" t="n">
+        <v>44732</v>
+      </c>
+      <c r="B150" t="n">
+        <v>0.6665000000000001</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="2" t="n">
+        <v>44733</v>
+      </c>
+      <c r="B151" t="n">
+        <v>0.993</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="2" t="n">
+        <v>44734</v>
+      </c>
+      <c r="B152" t="n">
+        <v>1.37655</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="2" t="n">
+        <v>44735</v>
+      </c>
+      <c r="B153" t="n">
+        <v>0.658</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="2" t="n">
+        <v>44736</v>
+      </c>
+      <c r="B154" t="n">
+        <v>0.414</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="2" t="n">
+        <v>44738</v>
+      </c>
+      <c r="B155" t="n">
+        <v>1.0918</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="2" t="n">
+        <v>44739</v>
+      </c>
+      <c r="B156" t="n">
+        <v>-0.5760000000000001</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="2" t="n">
+        <v>44740</v>
+      </c>
+      <c r="B157" t="n">
+        <v>0.83775</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="2" t="n">
+        <v>44741</v>
+      </c>
+      <c r="B158" t="n">
+        <v>1.164</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="2" t="n">
+        <v>44742</v>
+      </c>
+      <c r="B159" t="n">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="2" t="n">
+        <v>44743</v>
+      </c>
+      <c r="B160" t="n">
+        <v>0.993</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="2" t="n">
+        <v>44745</v>
+      </c>
+      <c r="B161" t="n">
+        <v>-0.06730000000000003</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="2" t="n">
+        <v>44746</v>
+      </c>
+      <c r="B162" t="n">
+        <v>1.2013</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="2" t="n">
+        <v>44747</v>
+      </c>
+      <c r="B163" t="n">
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="2" t="n">
+        <v>44748</v>
+      </c>
+      <c r="B164" t="n">
+        <v>0.9975000000000001</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="2" t="n">
+        <v>44749</v>
+      </c>
+      <c r="B165" t="n">
+        <v>0.527</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="2" t="n">
+        <v>44750</v>
+      </c>
+      <c r="B166" t="n">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="2" t="n">
+        <v>44753</v>
+      </c>
+      <c r="B167" t="n">
+        <v>0.9975000000000001</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="2" t="n">
+        <v>44754</v>
+      </c>
+      <c r="B168" t="n">
+        <v>1.09965</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="2" t="n">
+        <v>44755</v>
+      </c>
+      <c r="B169" t="n">
+        <v>0.9935</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="2" t="n">
+        <v>44756</v>
+      </c>
+      <c r="B170" t="n">
+        <v>0.996</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="2" t="n">
+        <v>44757</v>
+      </c>
+      <c r="B171" t="n">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="2" t="n">
+        <v>44758</v>
+      </c>
+      <c r="B172" t="n">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="2" t="n">
+        <v>44760</v>
+      </c>
+      <c r="B173" t="n">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="2" t="n">
+        <v>44761</v>
+      </c>
+      <c r="B174" t="n">
+        <v>0.988</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="2" t="n">
+        <v>44762</v>
+      </c>
+      <c r="B175" t="n">
+        <v>0.993</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="2" t="n">
+        <v>44763</v>
+      </c>
+      <c r="B176" t="n">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="2" t="n">
+        <v>44764</v>
+      </c>
+      <c r="B177" t="n">
+        <v>1.339</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="2" t="n">
+        <v>44766</v>
+      </c>
+      <c r="B178" t="n">
+        <v>0.9133</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="2" t="n">
+        <v>44767</v>
+      </c>
+      <c r="B179" t="n">
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="2" t="n">
+        <v>44768</v>
+      </c>
+      <c r="B180" t="n">
+        <v>-0.0503</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="2" t="n">
+        <v>44769</v>
+      </c>
+      <c r="B181" t="n">
+        <v>0.6685</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="2" t="n">
+        <v>44770</v>
+      </c>
+      <c r="B182" t="n">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="2" t="n">
+        <v>44771</v>
+      </c>
+      <c r="B183" t="n">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="2" t="n">
+        <v>44773</v>
+      </c>
+      <c r="B184" t="n">
+        <v>0.9486999999999999</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="2" t="n">
+        <v>44774</v>
+      </c>
+      <c r="B185" t="n">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="2" t="n">
+        <v>44775</v>
+      </c>
+      <c r="B186" t="n">
+        <v>1.09815</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="2" t="n">
+        <v>44776</v>
+      </c>
+      <c r="B187" t="n">
+        <v>0.9198</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="2" t="n">
+        <v>44777</v>
+      </c>
+      <c r="B188" t="n">
+        <v>0.8933</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="2" t="n">
+        <v>44778</v>
+      </c>
+      <c r="B189" t="n">
+        <v>1.0356</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="2" t="n">
+        <v>44780</v>
+      </c>
+      <c r="B190" t="n">
+        <v>-1.1869</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="2" t="n">
+        <v>44781</v>
+      </c>
+      <c r="B191" t="n">
+        <v>0.92145</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="2" t="n">
+        <v>44782</v>
+      </c>
+      <c r="B192" t="n">
+        <v>0.968</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="2" t="n">
+        <v>44783</v>
+      </c>
+      <c r="B193" t="n">
+        <v>0.4422</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="2" t="n">
+        <v>44784</v>
+      </c>
+      <c r="B194" t="n">
+        <v>0.3132</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="2" t="n">
+        <v>44785</v>
+      </c>
+      <c r="B195" t="n">
+        <v>0.696</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="2" t="n">
+        <v>44787</v>
+      </c>
+      <c r="B196" t="n">
+        <v>0.997</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="2" t="n">
+        <v>44788</v>
+      </c>
+      <c r="B197" t="n">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="B198" t="n">
+        <v>0.18965</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="2" t="n">
+        <v>44790</v>
+      </c>
+      <c r="B199" t="n">
+        <v>1.3896</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="2" t="n">
+        <v>44791</v>
+      </c>
+      <c r="B200" t="n">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="2" t="n">
+        <v>44792</v>
+      </c>
+      <c r="B201" t="n">
+        <v>0.86615</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="2" t="n">
+        <v>44795</v>
+      </c>
+      <c r="B202" t="n">
+        <v>1.1872</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="2" t="n">
+        <v>44796</v>
+      </c>
+      <c r="B203" t="n">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="2" t="n">
+        <v>44797</v>
+      </c>
+      <c r="B204" t="n">
+        <v>0.992</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="2" t="n">
+        <v>44798</v>
+      </c>
+      <c r="B205" t="n">
+        <v>0.90645</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="2" t="n">
+        <v>44799</v>
+      </c>
+      <c r="B206" t="n">
+        <v>0.9975000000000001</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="2" t="n">
+        <v>44802</v>
+      </c>
+      <c r="B207" t="n">
+        <v>0.5188999999999999</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="2" t="n">
+        <v>44803</v>
+      </c>
+      <c r="B208" t="n">
+        <v>1.5409</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="2" t="n">
+        <v>44804</v>
+      </c>
+      <c r="B209" t="n">
+        <v>0.1645</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="2" t="n">
+        <v>44805</v>
+      </c>
+      <c r="B210" t="n">
+        <v>0.958</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="2" t="n">
+        <v>44806</v>
+      </c>
+      <c r="B211" t="n">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="2" t="n">
+        <v>44809</v>
+      </c>
+      <c r="B212" t="n">
+        <v>1.31745</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="2" t="n">
+        <v>44810</v>
+      </c>
+      <c r="B213" t="n">
+        <v>0.985</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="2" t="n">
+        <v>44811</v>
+      </c>
+      <c r="B214" t="n">
+        <v>0.532</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="2" t="n">
+        <v>44812</v>
+      </c>
+      <c r="B215" t="n">
+        <v>0.839</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="2" t="n">
+        <v>44813</v>
+      </c>
+      <c r="B216" t="n">
+        <v>-0.39235</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="2" t="n">
+        <v>44814</v>
+      </c>
+      <c r="B217" t="n">
+        <v>1.2013</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="2" t="n">
+        <v>44815</v>
+      </c>
+      <c r="B218" t="n">
+        <v>-0.1917</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="2" t="n">
+        <v>44816</v>
+      </c>
+      <c r="B219" t="n">
+        <v>-1.40135</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="2" t="n">
+        <v>44817</v>
+      </c>
+      <c r="B220" t="n">
+        <v>0.12295</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="2" t="n">
+        <v>44818</v>
+      </c>
+      <c r="B221" t="n">
+        <v>0.994</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="2" t="n">
+        <v>44819</v>
+      </c>
+      <c r="B222" t="n">
+        <v>1.15995</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="2" t="n">
+        <v>44820</v>
+      </c>
+      <c r="B223" t="n">
+        <v>1.5096</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="2" t="n">
+        <v>44823</v>
+      </c>
+      <c r="B224" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="2" t="n">
+        <v>44824</v>
+      </c>
+      <c r="B225" t="n">
+        <v>0.6970000000000001</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="2" t="n">
+        <v>44825</v>
+      </c>
+      <c r="B226" t="n">
+        <v>1.5399</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="2" t="n">
+        <v>44826</v>
+      </c>
+      <c r="B227" t="n">
+        <v>0.998</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="2" t="n">
+        <v>44827</v>
+      </c>
+      <c r="B228" t="n">
+        <v>1.1305</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="2" t="n">
+        <v>44828</v>
+      </c>
+      <c r="B229" t="n">
+        <v>0.835</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test set predictions added
</commit_message>
<xml_diff>
--- a/Excel reports/adjusted_df_news.xlsx
+++ b/Excel reports/adjusted_df_news.xlsx
@@ -431,7 +431,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B43"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,338 +453,58 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>44550</v>
+        <v>44844</v>
       </c>
       <c r="B2" t="n">
-        <v>0.6143000000000001</v>
+        <v>0.75835</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44557</v>
+        <v>44851</v>
       </c>
       <c r="B3" t="n">
-        <v>0.5781000000000001</v>
+        <v>0.8032999999999999</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44564</v>
+        <v>44858</v>
       </c>
       <c r="B4" t="n">
-        <v>0.852</v>
+        <v>0.59615</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>44571</v>
+        <v>44865</v>
       </c>
       <c r="B5" t="n">
-        <v>0.995</v>
+        <v>0.53295</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>44578</v>
+        <v>44872</v>
       </c>
       <c r="B6" t="n">
-        <v>0.9924999999999999</v>
+        <v>0.5373</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>44585</v>
+        <v>44879</v>
       </c>
       <c r="B7" t="n">
-        <v>0.995</v>
+        <v>0.477</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>44592</v>
+        <v>44886</v>
       </c>
       <c r="B8" t="n">
-        <v>0.995</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
-        <v>44599</v>
-      </c>
-      <c r="B9" t="n">
-        <v>0.986</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
-        <v>44606</v>
-      </c>
-      <c r="B10" t="n">
-        <v>0.8704499999999999</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
-        <v>44613</v>
-      </c>
-      <c r="B11" t="n">
-        <v>0.9975000000000001</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="n">
-        <v>44620</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1.1598</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="n">
-        <v>44627</v>
-      </c>
-      <c r="B13" t="n">
-        <v>0.998</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="n">
-        <v>44634</v>
-      </c>
-      <c r="B14" t="n">
-        <v>0.19515</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="n">
-        <v>44641</v>
-      </c>
-      <c r="B15" t="n">
-        <v>0.86225</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="n">
-        <v>44648</v>
-      </c>
-      <c r="B16" t="n">
-        <v>0.957</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="n">
-        <v>44655</v>
-      </c>
-      <c r="B17" t="n">
-        <v>0.998</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="n">
-        <v>44662</v>
-      </c>
-      <c r="B18" t="n">
-        <v>0.967</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="n">
-        <v>44669</v>
-      </c>
-      <c r="B19" t="n">
-        <v>0.9804999999999999</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="n">
-        <v>44676</v>
-      </c>
-      <c r="B20" t="n">
-        <v>0.9895</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="n">
-        <v>44683</v>
-      </c>
-      <c r="B21" t="n">
-        <v>1.0248</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="n">
-        <v>44690</v>
-      </c>
-      <c r="B22" t="n">
-        <v>0.679</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="2" t="n">
-        <v>44697</v>
-      </c>
-      <c r="B23" t="n">
-        <v>0.999</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="2" t="n">
-        <v>44704</v>
-      </c>
-      <c r="B24" t="n">
-        <v>0.86465</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="2" t="n">
-        <v>44711</v>
-      </c>
-      <c r="B25" t="n">
-        <v>0.996</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="n">
-        <v>44718</v>
-      </c>
-      <c r="B26" t="n">
-        <v>0.956</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="2" t="n">
-        <v>44725</v>
-      </c>
-      <c r="B27" t="n">
-        <v>0.957</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="2" t="n">
-        <v>44732</v>
-      </c>
-      <c r="B28" t="n">
-        <v>0.988</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="2" t="n">
-        <v>44739</v>
-      </c>
-      <c r="B29" t="n">
-        <v>0.993</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="2" t="n">
-        <v>44746</v>
-      </c>
-      <c r="B30" t="n">
-        <v>0.98</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="2" t="n">
-        <v>44753</v>
-      </c>
-      <c r="B31" t="n">
-        <v>0.998</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="2" t="n">
-        <v>44760</v>
-      </c>
-      <c r="B32" t="n">
-        <v>0.997</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="2" t="n">
-        <v>44767</v>
-      </c>
-      <c r="B33" t="n">
-        <v>0.995</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="2" t="n">
-        <v>44774</v>
-      </c>
-      <c r="B34" t="n">
-        <v>0.90655</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="2" t="n">
-        <v>44781</v>
-      </c>
-      <c r="B35" t="n">
-        <v>0.7800499999999999</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="2" t="n">
-        <v>44788</v>
-      </c>
-      <c r="B36" t="n">
-        <v>0.9955000000000001</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="2" t="n">
-        <v>44795</v>
-      </c>
-      <c r="B37" t="n">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="2" t="n">
-        <v>44802</v>
-      </c>
-      <c r="B38" t="n">
-        <v>0.9924999999999999</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="2" t="n">
-        <v>44809</v>
-      </c>
-      <c r="B39" t="n">
-        <v>0.986</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="2" t="n">
-        <v>44816</v>
-      </c>
-      <c r="B40" t="n">
-        <v>0.993</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="2" t="n">
-        <v>44823</v>
-      </c>
-      <c r="B41" t="n">
-        <v>0.998</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="2" t="n">
-        <v>44830</v>
-      </c>
-      <c r="B42" t="n">
-        <v>0.9964999999999999</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="2" t="n">
-        <v>44837</v>
-      </c>
-      <c r="B43" t="n">
-        <v>1.0742</v>
+        <v>0.7139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>